<commit_message>
fixed ship highlighting, still need to fix sys diagrams and sim manager class
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/Ship_w_Series_Sys.xlsx
+++ b/shipClassTests/testResults/Ship_w_Series_Sys.xlsx
@@ -470,17 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="9" width="12.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -702,10 +696,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -724,116 +718,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <f>IF(B10 = E10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <f>IF(B11 = E11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <f>IF(B12 = E12, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3">
-        <f>IF(B13 = E13, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -849,7 +735,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1177,7 +1063,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1189,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1211,184 +1097,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
-        <v>1</v>
-      </c>
-      <c r="L10" s="3">
-        <f>IF(B10 = G10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
-        <v>1</v>
-      </c>
-      <c r="L11" s="3">
-        <f>IF(B11 = G11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3">
-        <f>IF(B12 = G12, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4">
-        <v>1</v>
-      </c>
-      <c r="L13" s="3">
-        <f>IF(B13 = G13, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
+  <conditionalFormatting sqref="E2:E10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L13">
+  <conditionalFormatting sqref="L2:L9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1404,7 +1134,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1738,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1759,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1789,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1810,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1840,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1861,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1874,252 +1604,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="3">
-        <f>IF(B10 = I10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="3">
-        <f>IF(B11 = I11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" s="4">
-        <v>1</v>
-      </c>
-      <c r="P12" s="3">
-        <f>IF(B12 = I12, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="3">
-        <f>IF(B13 = I13, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
+  <conditionalFormatting sqref="E2:E10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F14">
+  <conditionalFormatting sqref="F2:F10">
     <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="notContainsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(G2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K14">
+  <conditionalFormatting sqref="K2:K10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="6">
       <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L14">
+  <conditionalFormatting sqref="L2:L10">
     <cfRule type="notContainsBlanks" dxfId="0" priority="7">
       <formula>LEN(TRIM(L2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M14">
+  <conditionalFormatting sqref="M2:M10">
     <cfRule type="notContainsBlanks" dxfId="1" priority="8">
       <formula>LEN(TRIM(M2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N14">
+  <conditionalFormatting sqref="N2:N10">
     <cfRule type="notContainsBlanks" dxfId="1" priority="9">
       <formula>LEN(TRIM(N2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P13">
+  <conditionalFormatting sqref="P2:P9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>